<commit_message>
initial setup for 1-1 order
</commit_message>
<xml_diff>
--- a/BEERQL.xlsx
+++ b/BEERQL.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acbri\OneDrive - ASIAN INSTITUTE OF MANAGEMENT\0 DISS\code\beerql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF3509-F973-449C-8719-8F4715BC04FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608B71A2-D45C-4F0A-B752-6E5744276284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1010" yWindow="170" windowWidth="10250" windowHeight="5330" activeTab="1" xr2:uid="{D7081636-9A3B-467D-A133-C45D8070126A}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="31670" windowHeight="21070" xr2:uid="{D7081636-9A3B-467D-A133-C45D8070126A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Weekafter (2)" sheetId="4" r:id="rId1"/>
-    <sheet name="Weekafter" sheetId="1" r:id="rId2"/>
-    <sheet name="Exact, start at idx 0" sheetId="3" r:id="rId3"/>
-    <sheet name="PassOrder" sheetId="2" r:id="rId4"/>
+    <sheet name="Weekafter (4)" sheetId="6" r:id="rId1"/>
+    <sheet name="Weekafter (3)" sheetId="5" r:id="rId2"/>
+    <sheet name="Weekafter (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="Weekafter" sheetId="1" r:id="rId4"/>
+    <sheet name="Exact, start at idx 0" sheetId="3" r:id="rId5"/>
+    <sheet name="PassOrder" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="71">
   <si>
     <t>Period</t>
   </si>
@@ -83,6 +85,9 @@
     <t>-</t>
   </si>
   <si>
+    <t>15+3</t>
+  </si>
+  <si>
     <t>14+1</t>
   </si>
   <si>
@@ -174,16 +179,98 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">policy </t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>lead</t>
+  </si>
+  <si>
+    <t>4+12-15=1</t>
+  </si>
+  <si>
+    <t>0+12-0=12</t>
+  </si>
+  <si>
+    <t>computation</t>
+  </si>
+  <si>
+    <t>4+1-10=-5</t>
+  </si>
+  <si>
+    <t>0; 10+3</t>
+  </si>
+  <si>
+    <t>12+0-13=-1</t>
+  </si>
+  <si>
+    <t>0+12-2</t>
+  </si>
+  <si>
+    <t>Manufacturer --&gt;</t>
+  </si>
+  <si>
+    <t>2+0</t>
+  </si>
+  <si>
+    <t>2+2</t>
+  </si>
+  <si>
+    <t>0+12-2=10</t>
+  </si>
+  <si>
+    <t>2-5-8=-10</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>4+12+1-10=7</t>
+  </si>
+  <si>
+    <t>0+2</t>
+  </si>
+  <si>
+    <t>13+3</t>
+  </si>
+  <si>
+    <t>16+3</t>
+  </si>
+  <si>
+    <t>0+3</t>
+  </si>
+  <si>
+    <t>0+12-13=-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,6 +288,49 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -223,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -240,11 +370,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -266,20 +449,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -298,6 +530,104 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>49940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>396874</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>168529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{083C1984-4E48-4BAF-BB16-11B30AF45489}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3803649" y="6149115"/>
+          <a:ext cx="7083425" cy="2591914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>49940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>396874</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>168529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7C75D1D-20DA-4467-A129-4A044957E2F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3590924" y="6145940"/>
+          <a:ext cx="7067550" cy="2595089"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -346,7 +676,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -357,9 +687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
+      <xdr:colOff>149224</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>165354</xdr:rowOff>
+      <xdr:rowOff>168529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -395,20 +725,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>46765</xdr:rowOff>
+      <xdr:colOff>752474</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3176</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>165354</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>145682</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>22480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -431,8 +761,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="485774" y="2523265"/>
-          <a:ext cx="7000875" cy="2595089"/>
+          <a:off x="752474" y="4384676"/>
+          <a:ext cx="8816608" cy="3257804"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -740,11 +1070,1276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B10B73-B207-463C-862B-A7AC77BE0C4B}">
+  <dimension ref="A1:Y29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="6.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="15.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="1">
+        <v>2</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="1">
+        <v>4</v>
+      </c>
+      <c r="V1" s="3"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="30"/>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="3"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="X3" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="16">
+        <v>12</v>
+      </c>
+      <c r="K4" s="16">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="4">
+        <v>12</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="4">
+        <v>12</v>
+      </c>
+      <c r="U4" s="4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39">
+        <v>15</v>
+      </c>
+      <c r="B5" s="17">
+        <v>3</v>
+      </c>
+      <c r="C5" s="40">
+        <v>2</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="28">
+        <v>4</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0</v>
+      </c>
+      <c r="J5" s="41">
+        <v>12</v>
+      </c>
+      <c r="K5" s="40">
+        <v>1</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="28">
+        <v>0</v>
+      </c>
+      <c r="N5" s="28">
+        <v>0</v>
+      </c>
+      <c r="O5" s="22">
+        <v>12</v>
+      </c>
+      <c r="P5" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="28">
+        <v>0</v>
+      </c>
+      <c r="S5" s="28">
+        <v>0</v>
+      </c>
+      <c r="T5" s="22">
+        <v>12</v>
+      </c>
+      <c r="U5" s="17">
+        <v>3</v>
+      </c>
+      <c r="V5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="W5" s="28">
+        <v>0</v>
+      </c>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="17">
+        <f>IF(F5&gt;0, F5, -2*F5)+IF(J5&gt;0, J5, -2*J5)+IF(O5&gt;0, O5, -2*O5)+IF(T5&gt;0,T5, -2*T5)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>10</v>
+      </c>
+      <c r="B6" s="34">
+        <v>3</v>
+      </c>
+      <c r="C6" s="34">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34">
+        <v>4</v>
+      </c>
+      <c r="E6" s="35">
+        <v>2</v>
+      </c>
+      <c r="F6" s="34">
+        <v>-5</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="37">
+        <v>4</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="22">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="34">
+        <v>0</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="37">
+        <v>0</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="34">
+        <v>10</v>
+      </c>
+      <c r="P6" s="34">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="34">
+        <v>10</v>
+      </c>
+      <c r="U6" s="34">
+        <v>0</v>
+      </c>
+      <c r="V6" s="26"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="23">
+        <f>IF(F6&gt;0, F6, -2*F6)+IF(J6&gt;0, J6, -2*J6)+IF(O6&gt;0, O6, -2*O6)+IF(T6&gt;0,T6, -2*T6)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>8</v>
+      </c>
+      <c r="B7" s="34">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34">
+        <v>2</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35">
+        <v>3</v>
+      </c>
+      <c r="F7" s="34">
+        <v>0</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="34">
+        <v>4</v>
+      </c>
+      <c r="K7" s="34">
+        <v>0</v>
+      </c>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="34">
+        <v>1</v>
+      </c>
+      <c r="P7" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="34">
+        <v>10</v>
+      </c>
+      <c r="U7" s="34">
+        <v>2</v>
+      </c>
+      <c r="W7" s="21"/>
+      <c r="X7" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y7">
+        <f>IF(F7&gt;0, F7, -2*F7)+IF(J7&gt;0, J7, -2*J7)+IF(O7&gt;0, O7, -2*O7)+IF(T7&gt;0,T7, -2*T7)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>14</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1</v>
+      </c>
+      <c r="C8" s="34">
+        <v>4</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35">
+        <v>4</v>
+      </c>
+      <c r="F8" s="34">
+        <v>2</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="34">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="34">
+        <v>0</v>
+      </c>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="34">
+        <v>-6</v>
+      </c>
+      <c r="P8" s="34">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="34">
+        <v>-5</v>
+      </c>
+      <c r="U8" s="34">
+        <v>0</v>
+      </c>
+      <c r="W8" s="21"/>
+      <c r="X8" s="30"/>
+      <c r="Y8">
+        <f>IF(F8&gt;0, F8, -2*F8)+IF(J8&gt;0, J8, -2*J8)+IF(O8&gt;0, O8, -2*O8)+IF(T8&gt;0,T8, -2*T8)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <v>9</v>
+      </c>
+      <c r="B9" s="34">
+        <v>2</v>
+      </c>
+      <c r="C9" s="34">
+        <v>4</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35">
+        <v>5</v>
+      </c>
+      <c r="F9" s="34">
+        <v>-7</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="34">
+        <v>-16</v>
+      </c>
+      <c r="K9" s="34">
+        <v>1</v>
+      </c>
+      <c r="L9" s="36"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="34">
+        <v>-17</v>
+      </c>
+      <c r="P9" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="34">
+        <v>-18</v>
+      </c>
+      <c r="U9" s="34">
+        <v>0</v>
+      </c>
+      <c r="W9" s="21"/>
+      <c r="X9" s="30"/>
+      <c r="Y9">
+        <f>IF(F9&gt;0, F9, -2*F9)+IF(J9&gt;0, J9, -2*J9)+IF(O9&gt;0, O9, -2*O9)+IF(T9&gt;0,T9, -2*T9)</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>3</v>
+      </c>
+      <c r="B10" s="34">
+        <v>0</v>
+      </c>
+      <c r="C10" s="34">
+        <v>2</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35">
+        <v>6</v>
+      </c>
+      <c r="F10" s="34">
+        <v>0</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34">
+        <v>2</v>
+      </c>
+      <c r="W10" s="21"/>
+      <c r="X10" s="30"/>
+      <c r="Y10">
+        <f>IF(F10&gt;0, F10, -2*F10)+IF(J10&gt;0, J10, -2*J10)+IF(O10&gt;0, O10, -2*O10)+IF(T10&gt;0,T10, -2*T10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="E11" s="11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>-13</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="U11" s="34">
+        <v>0</v>
+      </c>
+      <c r="W11" s="21"/>
+      <c r="X11" s="30"/>
+      <c r="Y11">
+        <f>IF(F11&gt;0, F11, -2*F11)+IF(J11&gt;0, J11, -2*J11)+IF(O11&gt;0, O11, -2*O11)+IF(T11&gt;0,T11, -2*T11)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="30"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="30"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374D4417-E35A-40EF-B414-B34B3FCEEE2A}">
+  <dimension ref="A1:Y29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="6.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="15.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="1">
+        <v>2</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="1">
+        <v>4</v>
+      </c>
+      <c r="V1" s="3"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="30"/>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="3"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="X3" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="27">
+        <v>0</v>
+      </c>
+      <c r="I4" s="27"/>
+      <c r="J4" s="4">
+        <v>12</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8"/>
+      <c r="M4" s="27">
+        <v>0</v>
+      </c>
+      <c r="N4" s="27">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>12</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="27">
+        <v>0</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="4">
+        <v>12</v>
+      </c>
+      <c r="U4" s="4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>10</v>
+      </c>
+      <c r="B5" s="17">
+        <v>3</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="28">
+        <v>12</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="22">
+        <v>12</v>
+      </c>
+      <c r="K5" s="17">
+        <v>1</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="28">
+        <v>12</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" s="22">
+        <v>12</v>
+      </c>
+      <c r="P5" s="17">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="28">
+        <v>12</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" s="22">
+        <v>12</v>
+      </c>
+      <c r="U5" s="17">
+        <v>3</v>
+      </c>
+      <c r="V5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="W5" s="28"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="17">
+        <f>IF(F5&gt;0, F5, -2*F5)+IF(J5&gt;0, J5, -2*J5)+IF(O5&gt;0, O5, -2*O5)+IF(T5&gt;0,T5, -2*T5)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>8</v>
+      </c>
+      <c r="B6" s="23">
+        <v>3</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>4</v>
+      </c>
+      <c r="E6" s="24">
+        <v>2</v>
+      </c>
+      <c r="F6" s="22">
+        <v>-5</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="29">
+        <v>0</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="22">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="23">
+        <v>0</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="22">
+        <v>10</v>
+      </c>
+      <c r="P6" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29">
+        <v>2</v>
+      </c>
+      <c r="T6" s="22">
+        <v>10</v>
+      </c>
+      <c r="U6" s="23">
+        <v>0</v>
+      </c>
+      <c r="V6" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="W6" s="29">
+        <v>1</v>
+      </c>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="23">
+        <f>IF(F6&gt;0, F6, -2*F6)+IF(J6&gt;0, J6, -2*J6)+IF(O6&gt;0, O6, -2*O6)+IF(T6&gt;0,T6, -2*T6)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="W7" s="21"/>
+      <c r="X7" s="30"/>
+      <c r="Y7">
+        <f>IF(F7&gt;0, F7, -2*F7)+IF(J7&gt;0, J7, -2*J7)+IF(O7&gt;0, O7, -2*O7)+IF(T7&gt;0,T7, -2*T7)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8">
+        <v>-6</v>
+      </c>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T8">
+        <v>-5</v>
+      </c>
+      <c r="W8" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="X8" s="30"/>
+      <c r="Y8">
+        <f>IF(F8&gt;0, F8, -2*F8)+IF(J8&gt;0, J8, -2*J8)+IF(O8&gt;0, O8, -2*O8)+IF(T8&gt;0,T8, -2*T8)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>-7</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9">
+        <v>-16</v>
+      </c>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9">
+        <v>-17</v>
+      </c>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9">
+        <v>-18</v>
+      </c>
+      <c r="W9" s="21"/>
+      <c r="X9" s="30"/>
+      <c r="Y9">
+        <f>IF(F9&gt;0, F9, -2*F9)+IF(J9&gt;0, J9, -2*J9)+IF(O9&gt;0, O9, -2*O9)+IF(T9&gt;0,T9, -2*T9)</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="11">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="30"/>
+      <c r="Y10">
+        <f>IF(F10&gt;0, F10, -2*F10)+IF(J10&gt;0, J10, -2*J10)+IF(O10&gt;0, O10, -2*O10)+IF(T10&gt;0,T10, -2*T10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>-13</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="30"/>
+      <c r="Y11">
+        <f>IF(F11&gt;0, F11, -2*F11)+IF(J11&gt;0, J11, -2*J11)+IF(O11&gt;0, O11, -2*O11)+IF(T11&gt;0,T11, -2*T11)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="30"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="30"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65E9CD7-7622-4DC7-9048-ECEDA0CC02D7}">
   <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="10">
         <v>4</v>
@@ -989,7 +2584,7 @@
         <v>-5</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="10">
         <v>4</v>
@@ -1001,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -1043,10 +2638,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>4</v>
@@ -1055,10 +2650,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -1094,10 +2689,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J8">
         <v>-1</v>
@@ -1130,7 +2725,7 @@
         <v>-7</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J9">
         <v>-16</v>
@@ -1163,10 +2758,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X10">
         <f t="shared" si="0"/>
@@ -1190,7 +2785,7 @@
         <v>-13</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X11">
         <f t="shared" si="0"/>
@@ -1214,10 +2809,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1225,7 +2820,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1235,12 +2830,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3E59C7-5483-40E6-BD55-D6F47FFD467C}">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +2914,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -1431,7 +3026,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="10">
         <v>0</v>
@@ -1491,7 +3086,7 @@
         <v>-5</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6">
         <v>-1</v>
@@ -1500,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -1542,10 +3137,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>4</v>
@@ -1554,10 +3149,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -1593,10 +3188,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J8">
         <v>-1</v>
@@ -1629,7 +3224,7 @@
         <v>-7</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J9">
         <v>-16</v>
@@ -1662,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X10">
         <f t="shared" si="0"/>
@@ -1686,7 +3281,7 @@
         <v>-13</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X11">
         <f t="shared" si="0"/>
@@ -1710,12 +3305,29 @@
         <v>3</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="H13" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1725,12 +3337,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCCD03E-E47F-4487-9ABD-3370DE354ECF}">
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,10 +3530,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5">
         <v>12</v>
@@ -1975,7 +3587,7 @@
         <v>-5</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I6">
         <v>-1</v>
@@ -1984,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N6">
         <v>10</v>
@@ -2026,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>4</v>
@@ -2035,10 +3647,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -2074,7 +3686,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I8">
         <v>-1</v>
@@ -2158,7 +3770,7 @@
         <v>-13</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W11">
         <f t="shared" si="0"/>
@@ -2176,12 +3788,12 @@
         <v>3</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G13" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2191,12 +3803,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA625A-BF0C-4D6A-B8D0-E07EAAF0A537}">
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,19 +3826,19 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>

</xml_diff>